<commit_message>
csv to xlsv change in distance_matrix
</commit_message>
<xml_diff>
--- a/data/bcprovincial-coordinates.xlsx
+++ b/data/bcprovincial-coordinates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Varun\Documents\pyride\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{718DC2E4-CBA4-4717-9F06-32116739984D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{60FA9B9C-1E83-426D-800B-DA933E29AFB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3040" yWindow="3040" windowWidth="28800" windowHeight="15410" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bcprovincial-coordinates" sheetId="1" r:id="rId1"/>
@@ -2157,21 +2157,21 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="7" max="7" width="18.765625" customWidth="1"/>
-    <col min="8" max="8" width="22.15234375" customWidth="1"/>
-    <col min="9" max="9" width="41.921875" customWidth="1"/>
-    <col min="10" max="10" width="28.3046875" customWidth="1"/>
+    <col min="7" max="7" width="18.7265625" customWidth="1"/>
+    <col min="8" max="8" width="22.1796875" customWidth="1"/>
+    <col min="9" max="9" width="41.90625" customWidth="1"/>
+    <col min="10" max="10" width="28.26953125" customWidth="1"/>
     <col min="11" max="11" width="19" customWidth="1"/>
-    <col min="12" max="12" width="31.15234375" customWidth="1"/>
+    <col min="12" max="12" width="31.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>428</v>
       </c>
@@ -2209,7 +2209,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2226,7 +2226,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2264,7 +2264,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2302,7 +2302,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2340,7 +2340,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2378,7 +2378,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2416,7 +2416,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2454,7 +2454,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2471,7 +2471,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2509,7 +2509,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2547,7 +2547,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2585,7 +2585,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2623,7 +2623,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2661,7 +2661,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2678,7 +2678,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2716,7 +2716,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2754,7 +2754,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>16</v>
       </c>
@@ -2792,7 +2792,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>17</v>
       </c>
@@ -2830,7 +2830,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>18</v>
       </c>
@@ -2868,7 +2868,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>19</v>
       </c>
@@ -2906,7 +2906,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>20</v>
       </c>
@@ -2944,7 +2944,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>21</v>
       </c>
@@ -2982,7 +2982,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>22</v>
       </c>
@@ -3020,7 +3020,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>23</v>
       </c>
@@ -3058,7 +3058,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>24</v>
       </c>
@@ -3096,7 +3096,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>25</v>
       </c>
@@ -3134,7 +3134,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>26</v>
       </c>
@@ -3172,7 +3172,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>27</v>
       </c>
@@ -3210,7 +3210,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>28</v>
       </c>
@@ -3248,7 +3248,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>29</v>
       </c>
@@ -3286,7 +3286,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>30</v>
       </c>
@@ -3324,7 +3324,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>31</v>
       </c>
@@ -3362,7 +3362,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>32</v>
       </c>
@@ -3400,7 +3400,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>33</v>
       </c>
@@ -3438,7 +3438,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>34</v>
       </c>
@@ -3476,7 +3476,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>35</v>
       </c>
@@ -3493,7 +3493,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>36</v>
       </c>
@@ -3531,7 +3531,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>37</v>
       </c>
@@ -3569,7 +3569,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>38</v>
       </c>
@@ -3607,7 +3607,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>39</v>
       </c>
@@ -3645,7 +3645,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>40</v>
       </c>
@@ -3683,7 +3683,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>41</v>
       </c>
@@ -3721,7 +3721,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>42</v>
       </c>
@@ -3759,7 +3759,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>43</v>
       </c>
@@ -3797,7 +3797,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>44</v>
       </c>
@@ -3835,7 +3835,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>45</v>
       </c>
@@ -3873,7 +3873,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>46</v>
       </c>
@@ -3911,7 +3911,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>47</v>
       </c>
@@ -3949,7 +3949,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>48</v>
       </c>
@@ -3987,7 +3987,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>49</v>
       </c>
@@ -4025,7 +4025,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>50</v>
       </c>
@@ -4063,7 +4063,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>51</v>
       </c>
@@ -4101,7 +4101,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>52</v>
       </c>
@@ -4139,7 +4139,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>53</v>
       </c>
@@ -4177,7 +4177,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>54</v>
       </c>
@@ -4215,7 +4215,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>55</v>
       </c>
@@ -4253,7 +4253,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>56</v>
       </c>
@@ -4291,7 +4291,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>57</v>
       </c>
@@ -4329,7 +4329,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>58</v>
       </c>
@@ -4367,7 +4367,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>59</v>
       </c>
@@ -4405,7 +4405,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>60</v>
       </c>
@@ -4443,7 +4443,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>61</v>
       </c>
@@ -4481,7 +4481,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>62</v>
       </c>
@@ -4519,7 +4519,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>63</v>
       </c>
@@ -4557,7 +4557,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>64</v>
       </c>
@@ -4595,7 +4595,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>65</v>
       </c>
@@ -4633,7 +4633,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>66</v>
       </c>
@@ -4650,7 +4650,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>67</v>
       </c>
@@ -4688,7 +4688,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>68</v>
       </c>
@@ -4705,7 +4705,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>69</v>
       </c>
@@ -4743,7 +4743,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>70</v>
       </c>
@@ -4781,7 +4781,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>71</v>
       </c>
@@ -4819,7 +4819,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>72</v>
       </c>
@@ -4857,7 +4857,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>73</v>
       </c>
@@ -4895,7 +4895,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>74</v>
       </c>
@@ -4933,7 +4933,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>75</v>
       </c>
@@ -4971,7 +4971,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>76</v>
       </c>
@@ -5009,7 +5009,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>77</v>
       </c>
@@ -5047,7 +5047,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>78</v>
       </c>
@@ -5085,7 +5085,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>79</v>
       </c>
@@ -5123,7 +5123,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>80</v>
       </c>
@@ -5161,7 +5161,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>81</v>
       </c>
@@ -5199,7 +5199,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>82</v>
       </c>
@@ -5237,7 +5237,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>83</v>
       </c>
@@ -5275,7 +5275,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>84</v>
       </c>
@@ -5313,7 +5313,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>85</v>
       </c>

</xml_diff>